<commit_message>
Update vocabulary in passage details field
</commit_message>
<xml_diff>
--- a/PHA4GE to WHO and Sequence Repository Field Mappings.xlsx
+++ b/PHA4GE to WHO and Sequence Repository Field Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inesmendes/Documents/PHA4GE/SARS-CoV-2-Contextual-Data-Specification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmagriffiths/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8C2D17-B355-E34D-8B90-EB55AED2CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46D3764A-4255-C24D-B70A-4E3282C6F6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23900" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23900" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GISAID to PHA4GE field mappings" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="631">
   <si>
     <t>bioproject accession</t>
   </si>
@@ -303,12 +303,6 @@
   </si>
   <si>
     <t>e.g. Original, Vero</t>
-  </si>
-  <si>
-    <t>specimen processing; lab host; passage number; passage method</t>
-  </si>
-  <si>
-    <t>This field can be populated by the PHA4GE fields "specimen processing", "lab host", "passage number" and "passage method". If the information is unknown or can not be shared, put "unknown".</t>
   </si>
   <si>
     <t>Collection date</t>
@@ -2006,6 +2000,9 @@
   <si>
     <t>This field can be populated by the PHA4GE field "pre-existing conditions and risk factors".</t>
   </si>
+  <si>
+    <t xml:space="preserve">The submitter need only provide details in this field if the virus was passaged. If the genome was acquired from the sample without passaging in a cell line, then put "Original". If the information is unknown or can not be shared, put "unknown". If the virus was passaged, GISAID requires that the submitter use their controlled vocabulary for this field (e.g. Vero, Vero CCL81, Caco-2, LLC-MK2, C1, C2). Passages can be indicated as P1, P2 etc. Further GISAID documentation is available upon request to GISAID. </t>
+  </si>
 </sst>
 </file>
 
@@ -2189,7 +2186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2334,6 +2331,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2557,8 +2557,8 @@
   </sheetPr>
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2775,11 +2775,11 @@
       <c r="C6" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>76</v>
+      <c r="D6" s="70" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>77</v>
+        <v>630</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>61</v>
@@ -2818,7 +2818,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2845,19 +2845,19 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2884,17 +2884,17 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>61</v>
@@ -2933,7 +2933,7 @@
         <v>13</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -2960,17 +2960,17 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2997,17 +2997,17 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>61</v>
@@ -3046,7 +3046,7 @@
         <v>18</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -3073,10 +3073,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>61</v>
@@ -3085,7 +3085,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -3112,10 +3112,10 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>61</v>
@@ -3124,7 +3124,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -3151,17 +3151,17 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -3188,17 +3188,17 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -3225,17 +3225,17 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -3262,17 +3262,17 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -3299,10 +3299,10 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>61</v>
@@ -3311,7 +3311,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3338,17 +3338,17 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3375,17 +3375,17 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -3412,10 +3412,10 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>61</v>
@@ -3424,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="15" t="s">
@@ -3461,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3496,7 +3496,7 @@
         <v>34</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -3523,10 +3523,10 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>61</v>
@@ -3535,7 +3535,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="15" t="s">
@@ -3572,7 +3572,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3607,7 +3607,7 @@
         <v>28</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3634,17 +3634,17 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="18" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -31886,16 +31886,16 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>141</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>57</v>
@@ -31927,22 +31927,22 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -31968,22 +31968,22 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -32009,22 +32009,22 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -32050,22 +32050,22 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -32091,22 +32091,22 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -32132,22 +32132,22 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -32173,22 +32173,22 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -32214,22 +32214,22 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -32255,22 +32255,22 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -32296,22 +32296,22 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="E11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -32337,22 +32337,22 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="E12" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>179</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -32378,22 +32378,22 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="E13" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -32419,22 +32419,22 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -32460,7 +32460,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>16</v>
@@ -32469,13 +32469,13 @@
         <v>47</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -32501,13 +32501,13 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>61</v>
@@ -32516,7 +32516,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -32542,13 +32542,13 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>61</v>
@@ -32557,7 +32557,7 @@
         <v>19</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -32583,22 +32583,22 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -32624,7 +32624,7 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>14</v>
@@ -32639,7 +32639,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -32665,13 +32665,13 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>61</v>
@@ -32680,7 +32680,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -32706,13 +32706,13 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>61</v>
@@ -32721,7 +32721,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -32747,22 +32747,22 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>34</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -32788,13 +32788,13 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>61</v>
@@ -32803,7 +32803,7 @@
         <v>51</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -32829,13 +32829,13 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>61</v>
@@ -32844,7 +32844,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -32870,22 +32870,22 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B25" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -32911,22 +32911,22 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -32952,22 +32952,22 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>224</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -32993,22 +32993,22 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -33034,13 +33034,13 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>61</v>
@@ -33049,7 +33049,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -33075,22 +33075,22 @@
     </row>
     <row r="30" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>53</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -33116,22 +33116,22 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B31" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>233</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -33157,22 +33157,22 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B32" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -33198,22 +33198,22 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -33239,22 +33239,22 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -33280,22 +33280,22 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="B35" s="24" t="s">
-        <v>243</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -33321,22 +33321,22 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="D36" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -33391,16 +33391,16 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E38" s="21" t="s">
         <v>57</v>
@@ -33435,10 +33435,10 @@
         <v>35</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>61</v>
@@ -33447,7 +33447,7 @@
         <v>34</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -33473,13 +33473,13 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>61</v>
@@ -33488,7 +33488,7 @@
         <v>51</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -33514,13 +33514,13 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>61</v>
@@ -33529,7 +33529,7 @@
         <v>7</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -33555,13 +33555,13 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>61</v>
@@ -33570,7 +33570,7 @@
         <v>51</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -33596,13 +33596,13 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="25" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>61</v>
@@ -33635,13 +33635,13 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="25" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>61</v>
@@ -33650,7 +33650,7 @@
         <v>51</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -33676,13 +33676,13 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>61</v>
@@ -33691,7 +33691,7 @@
         <v>51</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -33717,13 +33717,13 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>61</v>
@@ -33732,7 +33732,7 @@
         <v>51</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -33758,13 +33758,13 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="25" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>61</v>
@@ -33773,7 +33773,7 @@
         <v>51</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -33799,13 +33799,13 @@
     </row>
     <row r="48" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>61</v>
@@ -33814,7 +33814,7 @@
         <v>51</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -33840,13 +33840,13 @@
     </row>
     <row r="49" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" s="25" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>61</v>
@@ -33855,7 +33855,7 @@
         <v>25</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -33888,7 +33888,7 @@
         <v>26</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -61316,14 +61316,14 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="52" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="36"/>
@@ -61335,16 +61335,16 @@
     </row>
     <row r="4" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E4" s="58" t="s">
         <v>57</v>
@@ -61380,19 +61380,19 @@
         <v>35</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E5" s="42" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61400,19 +61400,19 @@
         <v>32</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61420,19 +61420,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E7" s="42" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61440,39 +61440,39 @@
         <v>8</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61480,19 +61480,19 @@
         <v>37</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I10" s="7"/>
     </row>
@@ -61501,19 +61501,19 @@
         <v>38</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61521,99 +61521,99 @@
         <v>40</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="42" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>535</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="B13" s="42" t="s">
-        <v>537</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>353</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="42" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>535</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="B14" s="42" t="s">
-        <v>537</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>354</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="42" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>4</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="62" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>535</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="B16" s="62" t="s">
-        <v>537</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>359</v>
-      </c>
       <c r="D16" s="62" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E16" s="62" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="62" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G16" s="63"/>
       <c r="H16" s="63"/>
@@ -61621,22 +61621,22 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="62" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>535</v>
+      </c>
+      <c r="C17" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="B17" s="62" t="s">
-        <v>537</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>360</v>
-      </c>
       <c r="D17" s="62" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G17" s="63"/>
       <c r="H17" s="63"/>
@@ -61647,220 +61647,220 @@
         <v>39</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>303</v>
+      </c>
+      <c r="F18" s="37" t="s">
         <v>304</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>288</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>305</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>306</v>
       </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="42" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="42" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="42" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="42" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="36" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="42" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="64" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="42" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="42" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="42" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61868,39 +61868,39 @@
         <v>48</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E29" s="42" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="33" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E30" s="42" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61908,59 +61908,59 @@
         <v>46</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E31" s="42" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="42" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="42" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61968,19 +61968,19 @@
         <v>49</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>18</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -61988,393 +61988,393 @@
         <v>50</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="42" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="42" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>41</v>
       </c>
       <c r="F37" s="35" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="42" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>42</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="42" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D39" s="42" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="42" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E40" s="42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="42" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C41" s="30"/>
       <c r="D41" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F41" s="36" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="42" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E42" s="53" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="42" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E43" s="42" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="42" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F44" s="36" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="42" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F45" s="35" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="42" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E46" s="37" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F46" s="36" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="42" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E47" s="37" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F47" s="36" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="42" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E48" s="37" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F48" s="36" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="42" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C49" s="30"/>
       <c r="D49" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F49" s="36" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="42" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C50" s="30"/>
       <c r="D50" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E50" s="37" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F50" s="36" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="42" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B51" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E51" s="37" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F51" s="36" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="52" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="42" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C52" s="30"/>
       <c r="D52" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F52" s="36" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="42" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B53" s="42" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E53" s="42" t="s">
         <v>43</v>
       </c>
       <c r="F53" s="35" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="42" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E54" s="42" t="s">
         <v>44</v>
       </c>
       <c r="F54" s="35" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="61" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="2"/>
@@ -62391,14 +62391,14 @@
     </row>
     <row r="57" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B57" s="49"/>
       <c r="C57" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E57" s="31" t="s">
         <v>57</v>
@@ -62431,329 +62431,329 @@
     </row>
     <row r="58" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="32" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="32" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="60" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="32" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>51</v>
       </c>
       <c r="F60" s="36" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="43" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B61" s="50"/>
       <c r="C61" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F61" s="35" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="43" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B62" s="50"/>
       <c r="C62" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F62" s="35" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" s="43" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B63" s="50"/>
       <c r="C63" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F63" s="36" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="43" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B64" s="50"/>
       <c r="C64" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F64" s="36" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="43" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B65" s="50"/>
       <c r="C65" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F65" s="36" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="43" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B66" s="50"/>
       <c r="C66" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F66" s="36" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="48" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B67" s="46"/>
       <c r="C67" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F67" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="32" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="54" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F68" s="36" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B69" s="56"/>
       <c r="C69" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E69" s="40" t="s">
+        <v>426</v>
+      </c>
+      <c r="F69" s="41" t="s">
         <v>428</v>
-      </c>
-      <c r="F69" s="41" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="32" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="54"/>
       <c r="D70" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F70" s="38" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="53" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B71" s="53"/>
       <c r="C71" s="54"/>
       <c r="D71" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E71" s="35" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F71" s="38" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="53" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B72" s="53"/>
       <c r="C72" s="54"/>
       <c r="D72" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E72" s="35" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F72" s="37" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="53" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B73" s="53"/>
       <c r="C73" s="54"/>
       <c r="D73" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E73" s="35" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F73" s="37" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="53" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B74" s="53"/>
       <c r="C74" s="54"/>
       <c r="D74" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E74" s="36" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F74" s="37" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="53" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B75" s="53"/>
       <c r="C75" s="54"/>
       <c r="D75" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E75" s="35" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F75" s="37" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="51" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C76" s="51"/>
       <c r="D76" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E76" s="35" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F76" s="37" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -62763,7 +62763,7 @@
     </row>
     <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="49" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B78" s="49"/>
       <c r="E78" s="51"/>
@@ -62771,54 +62771,54 @@
     </row>
     <row r="79" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="47" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B79" s="46"/>
       <c r="C79" s="35" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E79" s="42" t="s">
         <v>34</v>
       </c>
       <c r="F79" s="36" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="44" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C80" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E80" s="42" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F80" s="37" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="44" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C81" s="35" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D81" s="37" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E81" s="42" t="s">
         <v>13</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="14" x14ac:dyDescent="0.15">
@@ -62826,103 +62826,103 @@
         <v>8</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E82" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="45" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E83" s="42" t="s">
         <v>6</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="44" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C84" s="35" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D84" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E84" s="46" t="s">
         <v>51</v>
       </c>
       <c r="F84" s="35" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A85" s="44" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C85" s="30" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E85" s="42" t="s">
         <v>1</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="44" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E86" s="42" t="s">
         <v>0</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="50" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B87" s="50"/>
       <c r="C87" s="20" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E87" s="34" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F87" s="37" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -62931,7 +62931,7 @@
     </row>
     <row r="89" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="49" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B89" s="49"/>
       <c r="E89" s="51"/>
@@ -62939,25 +62939,25 @@
     </row>
     <row r="90" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="44" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C90" s="35" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E90" s="42" t="s">
         <v>1</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N90" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="O90" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -62965,18 +62965,18 @@
         <v>35</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E91" s="42" t="s">
         <v>34</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="55" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B92" s="55"/>
       <c r="D92" s="37"/>
@@ -62985,67 +62985,67 @@
     </row>
     <row r="93" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="52" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B93" s="50"/>
       <c r="C93" s="35" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E93" s="46" t="s">
         <v>23</v>
       </c>
       <c r="F93" s="37" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="45" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B94" s="42"/>
       <c r="D94" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E94" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="F94" s="37" t="s">
         <v>438</v>
-      </c>
-      <c r="F94" s="37" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="52" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B95" s="50"/>
       <c r="D95" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E95" s="46" t="s">
+        <v>437</v>
+      </c>
+      <c r="F95" s="37" t="s">
         <v>439</v>
-      </c>
-      <c r="F95" s="37" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="44" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C96" s="36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E96" s="46" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F96" s="37" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="97" spans="5:6" ht="13" x14ac:dyDescent="0.15">
@@ -65892,7 +65892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B78A16-33A2-0347-91B5-D787CF857889}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -65907,13 +65907,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>541</v>
+      </c>
+      <c r="C1" s="67" t="s">
         <v>542</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>543</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>544</v>
       </c>
       <c r="D1" s="67" t="s">
         <v>57</v>
@@ -65924,456 +65924,456 @@
     </row>
     <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C2" s="69"/>
       <c r="D2" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="20" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A3" s="68" t="s">
+        <v>543</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>546</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="70" x14ac:dyDescent="0.15">
-      <c r="A3" s="68" t="s">
-        <v>545</v>
-      </c>
-      <c r="B3" s="63" t="s">
+      <c r="D3" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>549</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>550</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C5" s="69"/>
       <c r="D5" s="69" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C6" s="69"/>
       <c r="D6" s="69" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" s="69" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D8" s="69" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="140" x14ac:dyDescent="0.15">
+      <c r="A9" s="68" t="s">
+        <v>543</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>562</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="154" x14ac:dyDescent="0.15">
-      <c r="A9" s="68" t="s">
-        <v>545</v>
-      </c>
-      <c r="B9" s="63" t="s">
+      <c r="D9" s="69" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>564</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>565</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>349</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A10" s="68" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D10" s="69" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="68" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="69" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="69" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="68" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D12" s="69" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="68" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C13" s="69"/>
       <c r="D13" s="69" t="s">
+        <v>574</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A14" s="68" t="s">
+        <v>567</v>
+      </c>
+      <c r="B14" s="63" t="s">
         <v>576</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="84" x14ac:dyDescent="0.15">
-      <c r="A14" s="68" t="s">
-        <v>569</v>
-      </c>
-      <c r="B14" s="63" t="s">
+      <c r="D14" s="69" t="s">
         <v>578</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>579</v>
       </c>
-      <c r="D14" s="69" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="98" x14ac:dyDescent="0.15">
+      <c r="A15" s="68" t="s">
+        <v>567</v>
+      </c>
+      <c r="B15" s="63" t="s">
         <v>580</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="112" x14ac:dyDescent="0.15">
-      <c r="A15" s="68" t="s">
-        <v>569</v>
-      </c>
-      <c r="B15" s="63" t="s">
+      <c r="D15" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>583</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>584</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A16" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C16" s="69"/>
       <c r="D16" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C17" s="69"/>
       <c r="D17" s="69" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E17" s="11" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A18" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>589</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>590</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="84" x14ac:dyDescent="0.15">
-      <c r="A18" s="68" t="s">
-        <v>586</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>591</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>592</v>
       </c>
       <c r="D18" s="69" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="84" x14ac:dyDescent="0.15">
       <c r="A19" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B19" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>593</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>594</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>595</v>
       </c>
-      <c r="D19" s="11" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="B20" s="63" t="s">
         <v>596</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A20" s="68" t="s">
-        <v>586</v>
-      </c>
-      <c r="B20" s="63" t="s">
-        <v>598</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="69" t="s">
+        <v>597</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+      <c r="A21" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="B21" s="63" t="s">
         <v>599</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="98" x14ac:dyDescent="0.15">
-      <c r="A21" s="68" t="s">
-        <v>586</v>
-      </c>
-      <c r="B21" s="63" t="s">
+      <c r="D21" s="69" t="s">
         <v>601</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>602</v>
-      </c>
-      <c r="D21" s="69" t="s">
-        <v>603</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.15">
       <c r="A22" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B22" s="63" t="s">
+        <v>603</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="D22" s="69" t="s">
         <v>605</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>606</v>
       </c>
-      <c r="D22" s="69" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="98" x14ac:dyDescent="0.15">
+      <c r="A23" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="B23" s="63" t="s">
         <v>607</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="C23" s="69" t="s">
+        <v>604</v>
+      </c>
+      <c r="D23" s="69" t="s">
+        <v>607</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>608</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="112" x14ac:dyDescent="0.15">
-      <c r="A23" s="68" t="s">
-        <v>586</v>
-      </c>
-      <c r="B23" s="63" t="s">
-        <v>609</v>
-      </c>
-      <c r="C23" s="69" t="s">
-        <v>606</v>
-      </c>
-      <c r="D23" s="69" t="s">
-        <v>609</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D24" s="69" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="70" x14ac:dyDescent="0.15">
       <c r="A25" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C25" s="69"/>
       <c r="D25" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A26" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="B26" s="63" t="s">
         <v>615</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="84" x14ac:dyDescent="0.15">
-      <c r="A26" s="68" t="s">
-        <v>586</v>
-      </c>
-      <c r="B26" s="63" t="s">
+      <c r="D26" s="11" t="s">
         <v>617</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>618</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>619</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="70" x14ac:dyDescent="0.15">
       <c r="A27" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C27" s="69"/>
       <c r="D27" s="11" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A28" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B28" s="63" t="s">
+        <v>622</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>624</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>626</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="68" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B29" s="63" t="s">
+        <v>626</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="D29" s="69" t="s">
         <v>628</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="E29" s="11" t="s">
         <v>629</v>
-      </c>
-      <c r="D29" s="69" t="s">
-        <v>630</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>